<commit_message>
Created initial monte carlo simulation, base with fcff approximation, no capex, no NWC. Basic output of percentiles to show equity value per share.
</commit_message>
<xml_diff>
--- a/Costco Financial Model.xlsx
+++ b/Costco Financial Model.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Costco Financials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FA713A-9D89-4F9B-B4DC-EAEA3D9F646C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE8B95D7-BABE-4635-A8E4-3C3091A6A659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="350" windowWidth="22780" windowHeight="14800" activeTab="1" xr2:uid="{A1F3CBD5-A7CF-49C4-A7ED-958B12A488C4}"/>
   </bookViews>
@@ -993,9 +993,11 @@
     <v>4</v>
     <v>1078.2349999999999</v>
     <v>844.06</v>
-    <v>1.0016</v>
-    <v>-11.8101</v>
-    <v>-1.2411E-2</v>
+    <v>1.0017</v>
+    <v>-11.34</v>
+    <v>-1.3289999999999999E-3</v>
+    <v>-1.1917000000000001E-2</v>
+    <v>-1.25</v>
     <v>USD</v>
     <v>Costco Wholesale Corporation (Costco) operates membership warehouses and e-commerce sites that offer a selection of nationally branded and private-label products in a wide range of categories. The Company buys the majority of its merchandise directly from suppliers and route it to cross-docking consolidation points (depots) or directly to its warehouses. It operates 891 warehouses, including 614 in the United States and Puerto Rico, 108 in Canada, 40 in Mexico, 35 in Japan, 29 in the United Kingdom, 19 in Korea, 15 in Australia, 14 in Taiwan, seven in China, five in Spain, two in France, and one each in Iceland, New Zealand and Sweden. It also operates e-commerce sites in the United States, Canada, the United Kingdom, Mexico, Korea, Taiwan, Japan and Australia. The Company provides wide selection of merchandise, plus the convenience of specialty departments and exclusive member services.</v>
     <v>341000</v>
@@ -1003,23 +1005,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>999 Lake Dr, ISSAQUAH, WA, 98027- US</v>
-    <v>951.01</v>
+    <v>951.12</v>
     <v>Diversified Retail</v>
     <v>Stock</v>
-    <v>46052.814228171097</v>
+    <v>46053.041001608595</v>
     <v>0</v>
     <v>930.3</v>
-    <v>417139540345</v>
+    <v>417348203350</v>
     <v>COSTCO WHOLESALE CORPORATION</v>
     <v>COSTCO WHOLESALE CORPORATION</v>
     <v>948.83</v>
-    <v>50.341200000000001</v>
+    <v>50.366399999999999</v>
     <v>951.59</v>
-    <v>939.7799</v>
+    <v>940.25</v>
+    <v>939</v>
     <v>443869400</v>
     <v>COST</v>
     <v>COSTCO WHOLESALE CORPORATION (XNAS:COST)</v>
-    <v>1269273</v>
+    <v>2396325</v>
     <v>2520157</v>
     <v>1987</v>
   </rv>
@@ -1051,7 +1054,9 @@
     <k n="52 week low"/>
     <k n="Beta"/>
     <k n="Change"/>
+    <k n="Change % (Extended hours)"/>
     <k n="Change (%)"/>
+    <k n="Change (Extended hours)"/>
     <k n="Currency" t="s"/>
     <k n="Description" t="s"/>
     <k n="Employees"/>
@@ -1072,6 +1077,7 @@
     <k n="P/E"/>
     <k n="Previous close"/>
     <k n="Price"/>
+    <k n="Price (Extended hours)"/>
     <k n="Shares outstanding"/>
     <k n="Ticker symbol" t="s"/>
     <k n="UniqueName" t="s"/>
@@ -1088,7 +1094,7 @@
 <file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
 <supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
   <spbArrays count="1">
-    <a count="42">
+    <a count="45">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
       <v t="s">%IsRefreshable</v>
@@ -1099,13 +1105,16 @@
       <v t="s">Name</v>
       <v t="s">_SubLabel</v>
       <v t="s">Price</v>
+      <v t="s">Price (Extended hours)</v>
       <v t="s">Exchange</v>
       <v t="s">Official name</v>
       <v t="s">Last trade time</v>
       <v t="s">Ticker symbol</v>
       <v t="s">Exchange abbreviation</v>
       <v t="s">Change</v>
+      <v t="s">Change (Extended hours)</v>
       <v t="s">Change (%)</v>
+      <v t="s">Change % (Extended hours)</v>
       <v t="s">Currency</v>
       <v t="s">Previous close</v>
       <v t="s">Open</v>
@@ -1171,13 +1180,19 @@
       <v>8</v>
       <v>9</v>
       <v>4</v>
+      <v>1</v>
+      <v>1</v>
+      <v>5</v>
     </spb>
     <spb s="4">
-      <v>Real-Time Nasdaq Last Sale</v>
+      <v>at close</v>
       <v>from previous close</v>
       <v>from previous close</v>
-      <v>Source: Nasdaq Last Sale</v>
+      <v>Source: Nasdaq</v>
       <v>GMT</v>
+      <v>Delayed 15 minutes</v>
+      <v>from close</v>
+      <v>from close</v>
     </spb>
   </spbData>
 </supportingPropertyBags>
@@ -1222,6 +1237,9 @@
     <k n="Year incorporated" t="i"/>
     <k n="`%EntityServiceId" t="i"/>
     <k n="Shares outstanding" t="i"/>
+    <k n="Price (Extended hours)" t="i"/>
+    <k n="Change (Extended hours)" t="i"/>
+    <k n="Change % (Extended hours)" t="i"/>
   </s>
   <s>
     <k n="Price" t="s"/>
@@ -1229,6 +1247,9 @@
     <k n="Change (%)" t="s"/>
     <k n="ExchangeID" t="s"/>
     <k n="Last trade time" t="s"/>
+    <k n="Price (Extended hours)" t="s"/>
+    <k n="Change (Extended hours)" t="s"/>
+    <k n="Change % (Extended hours)" t="s"/>
   </s>
 </spbStructures>
 </file>
@@ -1609,8 +1630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B5F37E-9D1A-4503-B8AD-09D76B31B31A}">
   <dimension ref="A1:M112"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A26" zoomScale="121" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I93" sqref="I93"/>
+    <sheetView showGridLines="0" zoomScale="89" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1891,19 +1912,19 @@
       </c>
       <c r="J11" s="5">
         <f t="shared" ref="J11:M11" si="5">J33*I37</f>
-        <v>887.68842461727695</v>
+        <v>886.23344827820222</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" si="5"/>
-        <v>1176.5752989280534</v>
+        <v>1173.6941403784886</v>
       </c>
       <c r="L11" s="5">
         <f t="shared" si="5"/>
-        <v>1505.2456956993542</v>
+        <v>1501.0419293381046</v>
       </c>
       <c r="M11" s="5">
         <f t="shared" si="5"/>
-        <v>1881.0904735770328</v>
+        <v>1875.7767341437411</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -1976,19 +1997,19 @@
       </c>
       <c r="J13" s="6">
         <f t="shared" ref="J13" si="10">J9+J11+J12</f>
-        <v>12341.098138837893</v>
+        <v>12339.643162498818</v>
       </c>
       <c r="K13" s="6">
         <f t="shared" ref="K13" si="11">K9+K11+K12</f>
-        <v>13402.261865643313</v>
+        <v>13399.380707093747</v>
       </c>
       <c r="L13" s="6">
         <f t="shared" ref="L13" si="12">L9+L11+L12</f>
-        <v>14554.551772447774</v>
+        <v>14550.348006086526</v>
       </c>
       <c r="M13" s="6">
         <f t="shared" ref="M13" si="13">M9+M11+M12</f>
-        <v>15808.772090283719</v>
+        <v>15803.458350850427</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -2017,23 +2038,23 @@
       </c>
       <c r="I15" s="5">
         <f>-I23*I13</f>
-        <v>-2816.3758426109043</v>
+        <v>-2858.6460802639558</v>
       </c>
       <c r="J15" s="5">
         <f t="shared" ref="J15:M15" si="14">-J23*J13</f>
-        <v>-3054.2666344936342</v>
+        <v>-3099.7418190919007</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" si="14"/>
-        <v>-3316.8913157055053</v>
+        <v>-3365.9499047702438</v>
       </c>
       <c r="L15" s="5">
         <f t="shared" si="14"/>
-        <v>-3602.068580809731</v>
+        <v>-3655.0750781737747</v>
       </c>
       <c r="M15" s="5">
         <f t="shared" si="14"/>
-        <v>-3912.4723411537884</v>
+        <v>-3969.8587788407517</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -2062,23 +2083,23 @@
       </c>
       <c r="I16" s="6">
         <f>I13+I15</f>
-        <v>8563.4985524337862</v>
+        <v>8521.2283147807357</v>
       </c>
       <c r="J16" s="6">
         <f>J13+J15</f>
-        <v>9286.8315043442599</v>
+        <v>9239.9013434069166</v>
       </c>
       <c r="K16" s="6">
         <f>K13+K15</f>
-        <v>10085.370549937808</v>
+        <v>10033.430802323503</v>
       </c>
       <c r="L16" s="6">
         <f>L13+L15</f>
-        <v>10952.483191638043</v>
+        <v>10895.272927912751</v>
       </c>
       <c r="M16" s="6">
         <f t="shared" ref="M16" si="16">M13+M15</f>
-        <v>11896.29974912993</v>
+        <v>11833.599572009676</v>
       </c>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.3">
@@ -2244,24 +2265,24 @@
         <v>0.25134035866149013</v>
       </c>
       <c r="I23" s="10">
-        <f>AVERAGE(G23:H23)</f>
-        <v>0.24748742779070398</v>
+        <f>AVERAGE(F23:H23)</f>
+        <v>0.25120190091981498</v>
       </c>
       <c r="J23" s="10">
         <f>I23</f>
-        <v>0.24748742779070398</v>
+        <v>0.25120190091981498</v>
       </c>
       <c r="K23" s="10">
         <f t="shared" si="17"/>
-        <v>0.24748742779070398</v>
+        <v>0.25120190091981498</v>
       </c>
       <c r="L23" s="10">
         <f t="shared" si="17"/>
-        <v>0.24748742779070398</v>
+        <v>0.25120190091981498</v>
       </c>
       <c r="M23" s="10">
         <f t="shared" si="17"/>
-        <v>0.24748742779070398</v>
+        <v>0.25120190091981498</v>
       </c>
     </row>
     <row r="24" spans="3:13" x14ac:dyDescent="0.3">
@@ -2620,23 +2641,23 @@
       </c>
       <c r="I37" s="5">
         <f>I70-SUM(I38:I41)-I47</f>
-        <v>19321.497233666043</v>
+        <v>19289.828102323474</v>
       </c>
       <c r="J37" s="5">
         <f t="shared" ref="J37:M37" si="30">J70-SUM(J38:J41)-J47</f>
-        <v>25609.432040571555</v>
+        <v>25546.7205131917</v>
       </c>
       <c r="K37" s="5">
         <f t="shared" si="30"/>
-        <v>32763.298178617188</v>
+        <v>32671.798663846697</v>
       </c>
       <c r="L37" s="5">
         <f t="shared" si="30"/>
-        <v>40943.965668093944</v>
+        <v>40828.306390679085</v>
       </c>
       <c r="M37" s="5">
         <f t="shared" si="30"/>
-        <v>50383.314405249635</v>
+        <v>50251.40126007385</v>
       </c>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.3">
@@ -2825,23 +2846,23 @@
       </c>
       <c r="I42" s="6">
         <f t="shared" ref="I42:M42" si="33">SUM(I37:I41)</f>
-        <v>45318.885151858914</v>
+        <v>45287.216020516345</v>
       </c>
       <c r="J42" s="6">
         <f t="shared" si="33"/>
-        <v>53216.211559605617</v>
+        <v>53153.500032225762</v>
       </c>
       <c r="K42" s="6">
         <f t="shared" si="33"/>
-        <v>62168.308255626253</v>
+        <v>62076.808740855762</v>
       </c>
       <c r="L42" s="6">
         <f t="shared" si="33"/>
-        <v>72307.981361994622</v>
+        <v>72192.322084579762</v>
       </c>
       <c r="M42" s="6">
         <f t="shared" si="33"/>
-        <v>83791.11757657773</v>
+        <v>83659.204431401944</v>
       </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.3">
@@ -3044,23 +3065,23 @@
       </c>
       <c r="I49" s="6">
         <f>I42+I47</f>
-        <v>87314.118443908112</v>
+        <v>87282.449312565543</v>
       </c>
       <c r="J49" s="6">
         <f t="shared" ref="J49:M49" si="38">J42+J47</f>
-        <v>98705.489312570018</v>
+        <v>98642.777785190177</v>
       </c>
       <c r="K49" s="6">
         <f t="shared" si="38"/>
-        <v>111383.92220219434</v>
+        <v>111292.42268742385</v>
       </c>
       <c r="L49" s="6">
         <f t="shared" si="38"/>
-        <v>125497.66649829326</v>
+        <v>125382.00722087841</v>
       </c>
       <c r="M49" s="6">
         <f t="shared" si="38"/>
-        <v>141219.07886416832</v>
+        <v>141087.16571899253</v>
       </c>
     </row>
     <row r="51" spans="3:13" x14ac:dyDescent="0.3">
@@ -3204,23 +3225,23 @@
       </c>
       <c r="I54" s="5">
         <f t="shared" si="39"/>
-        <v>3560.3291189146694</v>
+        <v>3570.9302252251518</v>
       </c>
       <c r="J54" s="5">
         <f t="shared" si="39"/>
-        <v>4441.4658146432048</v>
+        <v>4467.9546858537333</v>
       </c>
       <c r="K54" s="5">
         <f t="shared" si="39"/>
-        <v>5540.6727647295947</v>
+        <v>5590.3133961637859</v>
       </c>
       <c r="L54" s="5">
         <f t="shared" si="39"/>
-        <v>6911.9196155025302</v>
+        <v>6994.6107480176361</v>
       </c>
       <c r="M54" s="5">
         <f t="shared" si="39"/>
-        <v>8622.5328222393637</v>
+        <v>8751.6702641138345</v>
       </c>
     </row>
     <row r="55" spans="3:13" x14ac:dyDescent="0.3">
@@ -3289,23 +3310,23 @@
       </c>
       <c r="I56" s="6">
         <f t="shared" ref="I56:M56" si="41">SUM(I51:I55)</f>
-        <v>40627.619891474329</v>
+        <v>40638.220997784811</v>
       </c>
       <c r="J56" s="6">
         <f t="shared" si="41"/>
-        <v>44569.159255791979</v>
+        <v>44595.648127002511</v>
       </c>
       <c r="K56" s="6">
         <f t="shared" si="41"/>
-        <v>48999.221595478499</v>
+        <v>49048.862226912694</v>
       </c>
       <c r="L56" s="6">
         <f t="shared" si="41"/>
-        <v>53997.48269993937</v>
+        <v>54080.173832454486</v>
       </c>
       <c r="M56" s="6">
         <f t="shared" si="41"/>
-        <v>59659.59531668447</v>
+        <v>59788.732758558937</v>
       </c>
     </row>
     <row r="58" spans="3:13" x14ac:dyDescent="0.3">
@@ -3493,23 +3514,23 @@
       </c>
       <c r="I62" s="6">
         <f>SUM(I58:I61)+I56</f>
-        <v>51454.619891474329</v>
+        <v>51465.220997784811</v>
       </c>
       <c r="J62" s="6">
         <f t="shared" ref="J62" si="47">SUM(J58:J61)+J56</f>
-        <v>55396.159255791979</v>
+        <v>55422.648127002511</v>
       </c>
       <c r="K62" s="6">
         <f t="shared" ref="K62:L62" si="48">SUM(K58:K61)+K56</f>
-        <v>59826.221595478499</v>
+        <v>59875.862226912694</v>
       </c>
       <c r="L62" s="6">
         <f t="shared" si="48"/>
-        <v>64824.48269993937</v>
+        <v>64907.173832454486</v>
       </c>
       <c r="M62" s="6">
         <f t="shared" ref="M62" si="49">SUM(M58:M61)+M56</f>
-        <v>70486.59531668447</v>
+        <v>70615.732758558937</v>
       </c>
     </row>
     <row r="64" spans="3:13" x14ac:dyDescent="0.3">
@@ -3653,23 +3674,23 @@
       </c>
       <c r="I67" s="5">
         <f>I86</f>
-        <v>28905.498552433786</v>
+        <v>28863.228314780736</v>
       </c>
       <c r="J67" s="5">
         <f t="shared" ref="J67:M67" si="53">J86</f>
-        <v>35884.330056778046</v>
+        <v>35795.129658187652</v>
       </c>
       <c r="K67" s="5">
         <f t="shared" si="53"/>
-        <v>43661.700606715851</v>
+        <v>43520.560460511158</v>
       </c>
       <c r="L67" s="5">
         <f t="shared" si="53"/>
-        <v>52306.183798353894</v>
+        <v>52107.833388423911</v>
       </c>
       <c r="M67" s="5">
         <f t="shared" si="53"/>
-        <v>61894.483547483826</v>
+        <v>61633.432960433587</v>
       </c>
     </row>
     <row r="68" spans="2:13" x14ac:dyDescent="0.3">
@@ -3698,23 +3719,23 @@
       </c>
       <c r="I68" s="6">
         <f t="shared" ref="I68:M68" si="55">SUM(I64:I67)</f>
-        <v>35859.498552433783</v>
+        <v>35817.228314780732</v>
       </c>
       <c r="J68" s="6">
         <f t="shared" si="55"/>
-        <v>43309.330056778046</v>
+        <v>43220.129658187652</v>
       </c>
       <c r="K68" s="6">
         <f t="shared" si="55"/>
-        <v>51557.700606715851</v>
+        <v>51416.560460511158</v>
       </c>
       <c r="L68" s="6">
         <f t="shared" si="55"/>
-        <v>60673.183798353894</v>
+        <v>60474.833388423911</v>
       </c>
       <c r="M68" s="6">
         <f t="shared" si="55"/>
-        <v>70732.483547483833</v>
+        <v>70471.432960433594</v>
       </c>
     </row>
     <row r="69" spans="2:13" x14ac:dyDescent="0.3">
@@ -3748,23 +3769,23 @@
       </c>
       <c r="I70" s="6">
         <f t="shared" si="57"/>
-        <v>87314.118443908112</v>
+        <v>87282.449312565543</v>
       </c>
       <c r="J70" s="6">
         <f t="shared" ref="J70:M70" si="58">J68+J62</f>
-        <v>98705.489312570018</v>
+        <v>98642.777785190163</v>
       </c>
       <c r="K70" s="6">
         <f t="shared" si="58"/>
-        <v>111383.92220219434</v>
+        <v>111292.42268742385</v>
       </c>
       <c r="L70" s="6">
         <f t="shared" si="58"/>
-        <v>125497.66649829326</v>
+        <v>125382.0072208784</v>
       </c>
       <c r="M70" s="6">
         <f t="shared" si="58"/>
-        <v>141219.07886416832</v>
+        <v>141087.16571899253</v>
       </c>
     </row>
     <row r="71" spans="2:13" x14ac:dyDescent="0.3">
@@ -3793,23 +3814,23 @@
       </c>
       <c r="I71" s="5">
         <f t="shared" si="60"/>
-        <v>87314.118443908112</v>
+        <v>87282.449312565543</v>
       </c>
       <c r="J71" s="5">
         <f t="shared" ref="J71:M71" si="61">J49</f>
-        <v>98705.489312570018</v>
+        <v>98642.777785190177</v>
       </c>
       <c r="K71" s="5">
         <f t="shared" si="61"/>
-        <v>111383.92220219434</v>
+        <v>111292.42268742385</v>
       </c>
       <c r="L71" s="5">
         <f t="shared" si="61"/>
-        <v>125497.66649829326</v>
+        <v>125382.00722087841</v>
       </c>
       <c r="M71" s="5">
         <f t="shared" si="61"/>
-        <v>141219.07886416832</v>
+        <v>141087.16571899253</v>
       </c>
     </row>
     <row r="72" spans="2:13" x14ac:dyDescent="0.3">
@@ -4033,19 +4054,19 @@
       </c>
       <c r="J83" s="5">
         <f>I86</f>
-        <v>28905.498552433786</v>
+        <v>28863.228314780736</v>
       </c>
       <c r="K83" s="5">
         <f>J86</f>
-        <v>35884.330056778046</v>
+        <v>35795.129658187652</v>
       </c>
       <c r="L83" s="5">
         <f>K86</f>
-        <v>43661.700606715851</v>
+        <v>43520.560460511158</v>
       </c>
       <c r="M83" s="5">
         <f>L86</f>
-        <v>52306.183798353894</v>
+        <v>52107.833388423911</v>
       </c>
     </row>
     <row r="84" spans="2:13" x14ac:dyDescent="0.3">
@@ -4054,23 +4075,23 @@
       </c>
       <c r="I84" s="5">
         <f>I16</f>
-        <v>8563.4985524337862</v>
+        <v>8521.2283147807357</v>
       </c>
       <c r="J84" s="5">
         <f>J16</f>
-        <v>9286.8315043442599</v>
+        <v>9239.9013434069166</v>
       </c>
       <c r="K84" s="5">
         <f>K16</f>
-        <v>10085.370549937808</v>
+        <v>10033.430802323503</v>
       </c>
       <c r="L84" s="5">
         <f>L16</f>
-        <v>10952.483191638043</v>
+        <v>10895.272927912751</v>
       </c>
       <c r="M84" s="5">
         <f>M16</f>
-        <v>11896.29974912993</v>
+        <v>11833.599572009676</v>
       </c>
     </row>
     <row r="85" spans="2:13" x14ac:dyDescent="0.3">
@@ -4104,23 +4125,23 @@
       <c r="H86" s="4"/>
       <c r="I86" s="6">
         <f>SUM(I83:I85)</f>
-        <v>28905.498552433786</v>
+        <v>28863.228314780736</v>
       </c>
       <c r="J86" s="6">
         <f>SUM(J83:J85)</f>
-        <v>35884.330056778046</v>
+        <v>35795.129658187652</v>
       </c>
       <c r="K86" s="6">
         <f t="shared" ref="K86:M86" si="72">SUM(K83:K85)</f>
-        <v>43661.700606715851</v>
+        <v>43520.560460511158</v>
       </c>
       <c r="L86" s="6">
         <f t="shared" si="72"/>
-        <v>52306.183798353894</v>
+        <v>52107.833388423911</v>
       </c>
       <c r="M86" s="6">
         <f t="shared" si="72"/>
-        <v>61894.483547483826</v>
+        <v>61633.432960433587</v>
       </c>
     </row>
     <row r="89" spans="2:13" x14ac:dyDescent="0.3">
@@ -4156,23 +4177,23 @@
       </c>
       <c r="I91" s="6">
         <f t="shared" si="73"/>
-        <v>5160.497233666043</v>
+        <v>5128.828102323474</v>
       </c>
       <c r="J91" s="6">
         <f t="shared" si="73"/>
-        <v>6287.9348069055122</v>
+        <v>6256.8924108682259</v>
       </c>
       <c r="K91" s="6">
         <f t="shared" si="73"/>
-        <v>7153.8661380456324</v>
+        <v>7125.0781506549974</v>
       </c>
       <c r="L91" s="6">
         <f t="shared" si="73"/>
-        <v>8180.6674894767566</v>
+        <v>8156.5077268323876</v>
       </c>
       <c r="M91" s="6">
         <f t="shared" si="73"/>
-        <v>9439.3487371556912</v>
+        <v>9423.0948693947648</v>
       </c>
     </row>
     <row r="93" spans="2:13" x14ac:dyDescent="0.3">
@@ -4397,8 +4418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE05CD12-7AD9-4955-8F5F-850ED1B91DAF}">
   <dimension ref="A1:P94"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A53" zoomScale="85" workbookViewId="0">
-      <selection activeCell="M94" sqref="M94"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A48" zoomScale="99" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -4433,14 +4454,14 @@
       </c>
       <c r="G4" s="57">
         <f ca="1">N83</f>
-        <v>425.95404454149326</v>
+        <v>426.11015988054891</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>129</v>
       </c>
       <c r="L4" s="24">
         <f ca="1">G4/G5-1</f>
-        <v>-0.54675127171639515</v>
+        <v>-0.54681184803983096</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -4449,14 +4470,14 @@
       </c>
       <c r="C5" s="16">
         <f ca="1">TODAY()</f>
-        <v>46052</v>
+        <v>46054</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>127</v>
       </c>
       <c r="G5" s="57" cm="1">
         <f t="array" aca="1" ref="G5" ca="1">_FV(C4,"price")</f>
-        <v>939.7799</v>
+        <v>940.25</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -4935,23 +4956,23 @@
       </c>
       <c r="J26" s="5">
         <f>'3_Statement_Model'!I15</f>
-        <v>-2816.3758426109043</v>
+        <v>-2858.6460802639558</v>
       </c>
       <c r="K26" s="5">
         <f>'3_Statement_Model'!J15</f>
-        <v>-3054.2666344936342</v>
+        <v>-3099.7418190919007</v>
       </c>
       <c r="L26" s="5">
         <f>'3_Statement_Model'!K15</f>
-        <v>-3316.8913157055053</v>
+        <v>-3365.9499047702438</v>
       </c>
       <c r="M26" s="5">
         <f>'3_Statement_Model'!L15</f>
-        <v>-3602.068580809731</v>
+        <v>-3655.0750781737747</v>
       </c>
       <c r="N26" s="5">
         <f>'3_Statement_Model'!M15</f>
-        <v>-3912.4723411537884</v>
+        <v>-3969.8587788407517</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
@@ -4982,23 +5003,23 @@
       </c>
       <c r="J27" s="9">
         <f t="shared" si="3"/>
-        <v>-0.25856904230970273</v>
+        <v>-0.26244983645045233</v>
       </c>
       <c r="K27" s="9">
         <f t="shared" si="3"/>
-        <v>-0.26292946421109514</v>
+        <v>-0.26684423896791831</v>
       </c>
       <c r="L27" s="9">
         <f t="shared" si="3"/>
-        <v>-0.26773795507673676</v>
+        <v>-0.27169794202383674</v>
       </c>
       <c r="M27" s="9">
         <f t="shared" si="3"/>
-        <v>-0.27263215106933525</v>
+        <v>-0.27664408895247289</v>
       </c>
       <c r="N27" s="9">
         <f t="shared" si="3"/>
-        <v>-0.27766603934386225</v>
+        <v>-0.28173872369155362</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
@@ -6226,7 +6247,7 @@
         <v>6594.8306598391309</v>
       </c>
       <c r="N69" s="28">
-        <f t="shared" ca="1" si="31"/>
+        <f ca="1">N58-N60+N63-N66</f>
         <v>7495.9036093973864</v>
       </c>
     </row>
@@ -6237,23 +6258,23 @@
       <c r="I70" s="33"/>
       <c r="J70" s="1">
         <f ca="1">J69/(1+wacc)^J74</f>
-        <v>4249.6792922976583</v>
+        <v>4251.3191783160928</v>
       </c>
       <c r="K70" s="1">
         <f ca="1">K69/(1+wacc)^K74</f>
-        <v>4927.1277364873304</v>
+        <v>4929.029039463474</v>
       </c>
       <c r="L70" s="1">
         <f ca="1">L69/(1+wacc)^L74</f>
-        <v>5191.5574083235115</v>
+        <v>5193.5607506517745</v>
       </c>
       <c r="M70" s="1">
         <f ca="1">M69/(1+wacc)^M74</f>
-        <v>5338.6597430409111</v>
+        <v>5340.7198499025399</v>
       </c>
       <c r="N70" s="1">
         <f ca="1">N69/(1+wacc)^N74</f>
-        <v>5655.535778391838</v>
+        <v>5657.7181628523649</v>
       </c>
     </row>
     <row r="71" spans="2:14" x14ac:dyDescent="0.3">
@@ -6266,7 +6287,7 @@
       <c r="I72" s="33"/>
       <c r="J72" s="54">
         <f ca="1">(DATE(YEAR(C5),12,31)-C5)/365</f>
-        <v>0.9178082191780822</v>
+        <v>0.9123287671232877</v>
       </c>
     </row>
     <row r="73" spans="2:14" x14ac:dyDescent="0.3">
@@ -6301,23 +6322,23 @@
       <c r="I74" s="33"/>
       <c r="J74" s="54">
         <f ca="1">J73*J72</f>
-        <v>0.9178082191780822</v>
+        <v>0.9123287671232877</v>
       </c>
       <c r="K74" s="54">
         <f ca="1">J72+(1/12)</f>
-        <v>1.0011415525114156</v>
+        <v>0.99566210045662107</v>
       </c>
       <c r="L74" s="54">
         <f ca="1">K74+1</f>
-        <v>2.0011415525114158</v>
+        <v>1.9956621004566211</v>
       </c>
       <c r="M74" s="54">
         <f t="shared" ref="M74:N74" ca="1" si="33">L74+1</f>
-        <v>3.0011415525114158</v>
+        <v>2.9956621004566211</v>
       </c>
       <c r="N74" s="54">
         <f t="shared" ca="1" si="33"/>
-        <v>4.0011415525114158</v>
+        <v>3.9956621004566211</v>
       </c>
     </row>
     <row r="75" spans="2:14" x14ac:dyDescent="0.3">
@@ -6340,7 +6361,7 @@
       <c r="I77" s="33"/>
       <c r="N77" s="5">
         <f ca="1">N76/(wacc+1)^N74</f>
-        <v>154248.42361014464</v>
+        <v>154307.94570954214</v>
       </c>
     </row>
     <row r="78" spans="2:14" x14ac:dyDescent="0.3">
@@ -6350,7 +6371,7 @@
       <c r="I78" s="33"/>
       <c r="N78" s="5">
         <f ca="1">SUM(J70:N70)+N77</f>
-        <v>179610.98356868589</v>
+        <v>179680.29269072838</v>
       </c>
     </row>
     <row r="79" spans="2:14" x14ac:dyDescent="0.3">
@@ -6380,7 +6401,7 @@
       <c r="I81" s="33"/>
       <c r="N81" s="5">
         <f ca="1">N78+N79-N80</f>
-        <v>189106.98356868589</v>
+        <v>189176.29269072838</v>
       </c>
     </row>
     <row r="82" spans="2:14" x14ac:dyDescent="0.3">
@@ -6409,7 +6430,7 @@
       <c r="M83" s="50"/>
       <c r="N83" s="56">
         <f ca="1">N81/N82</f>
-        <v>425.95404454149326</v>
+        <v>426.11015988054891</v>
       </c>
     </row>
     <row r="84" spans="2:14" x14ac:dyDescent="0.3">

</xml_diff>